<commit_message>
Arreglada errata competitor analysis
</commit_message>
<xml_diff>
--- a/P1/Competitor Analysis.xlsx
+++ b/P1/Competitor Analysis.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Multiple Competitor Feature Com" sheetId="1" r:id="rId4"/>
+    <sheet name="Multiple Competitor Feature Com" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t>Competitor Feature Comparison Card</t>
+    <t xml:space="preserve">Competitor Feature Comparison Card</t>
   </si>
   <si>
     <t>Lambus</t>
@@ -22,115 +24,115 @@
     <t>Tripit</t>
   </si>
   <si>
-    <t>Sygic Travel</t>
+    <t xml:space="preserve">Sygic Travel</t>
   </si>
   <si>
     <t>Polarsteps</t>
   </si>
   <si>
-    <t>Servicio Web</t>
+    <t xml:space="preserve">Servicio Web</t>
   </si>
   <si>
-    <t>La plataforma se puede utilizar desde el navegador web</t>
+    <t xml:space="preserve">La plataforma se puede utilizar desde el navegador web</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>✓</t>
   </si>
   <si>
-    <t>X</t>
+    <t xml:space="preserve">App móvil</t>
   </si>
   <si>
-    <t>App móvil</t>
-  </si>
-  <si>
-    <t>La plataforma dispone de una app móvil</t>
+    <t xml:space="preserve">La plataforma dispone de una app móvil</t>
   </si>
   <si>
     <t>Gratuito</t>
   </si>
   <si>
-    <t>El usuario dispone de la funcionalidad completa de la aplicación de forma gratuita</t>
+    <t xml:space="preserve">El usuario dispone de la funcionalidad completa de la aplicación de forma gratuita</t>
   </si>
   <si>
-    <t>Control de gastos</t>
+    <t xml:space="preserve">Control de gastos</t>
   </si>
   <si>
-    <t>Recoge los gastos de grupo, individuales y las deudas entre los componentes del viaje</t>
+    <t xml:space="preserve">Recoge los gastos de grupo, individuales y las deudas entre los componentes del viaje</t>
   </si>
   <si>
-    <t>Plan de Viaje</t>
+    <t xml:space="preserve">Plan de Viaje</t>
   </si>
   <si>
-    <t>Permite crear un listado de los lugares a visitar y su fecha de visita</t>
+    <t xml:space="preserve">Permite crear un listado de los lugares a visitar y su fecha de visita</t>
   </si>
   <si>
-    <t>Recomendaciones Inteligentes</t>
+    <t xml:space="preserve">Recomendaciones Inteligentes</t>
   </si>
   <si>
-    <t>Capacidad de realizar recomendaciones personalizadas al viajero según sus intereses y viajes pasados</t>
+    <t xml:space="preserve">Capacidad de realizar recomendaciones personalizadas al viajero según sus intereses y viajes pasados</t>
   </si>
   <si>
-    <t>Gestión de documentos de viaje</t>
+    <t xml:space="preserve">Gestión de documentos de viaje</t>
   </si>
   <si>
-    <t>Almacén para mantener ordenados documentos importantes del viaje como tickets o reservas</t>
+    <t xml:space="preserve">Almacén para mantener ordenados documentos importantes del viaje como tickets o reservas</t>
   </si>
   <si>
-    <t>Modo offline</t>
+    <t xml:space="preserve">Modo offline</t>
   </si>
   <si>
-    <t>Posibilidad de acceder a las planificaciones y documentos del usuario o mapas sin conexión a internet</t>
+    <t xml:space="preserve">Posibilidad de acceder a las planificaciones y documentos del usuario o mapas sin conexión a internet</t>
   </si>
   <si>
     <t>Notas</t>
   </si>
   <si>
-    <t>Información adicional sobre el viaje que puede ser compartida a otros miembros del grupo o ser privada</t>
+    <t xml:space="preserve">Información adicional sobre el viaje que puede ser compartida a otros miembros del grupo o ser privada</t>
   </si>
   <si>
-    <t>Información COVID-19</t>
+    <t xml:space="preserve">Información COVID-19</t>
   </si>
   <si>
-    <t>Informa de las restricciones actuales por COVID-19 en el lugar de destino</t>
+    <t xml:space="preserve">Informa de las restricciones actuales por COVID-19 en el lugar de destino</t>
   </si>
   <si>
-    <t>Información sobre huella de carbono</t>
+    <t xml:space="preserve">Información sobre huella de carbono</t>
   </si>
   <si>
-    <t>Muestra comparativas sobre la huella de carbono de las distintas opciones de vuelo</t>
+    <t xml:space="preserve">Muestra comparativas sobre la huella de carbono de las distintas opciones de vuelo</t>
   </si>
   <si>
-    <t>Seguridad del destino</t>
+    <t xml:space="preserve">Seguridad del destino</t>
   </si>
   <si>
     <t xml:space="preserve">Puntuación de la seguridad de la ciudad o barrio según estadísticas como número de robos, asesinatos, inclusión LGTB, etc. </t>
   </si>
   <si>
-    <t>Recomendaciones Locales</t>
+    <t xml:space="preserve">Recomendaciones Locales</t>
   </si>
   <si>
-    <t>Recomienda lugares turísticos típicos del sitio al que se viaja</t>
+    <t xml:space="preserve">Recomienda lugares turísticos típicos del sitio al que se viaja</t>
   </si>
   <si>
     <r>
       <rPr>
+        <color theme="1"/>
         <rFont val="Avenir"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">Copy this cell for when you or a competitor </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Avenir"/>
         <i/>
         <color theme="1"/>
+        <rFont val="Avenir"/>
       </rPr>
       <t>does</t>
     </r>
     <r>
       <rPr>
+        <color theme="1"/>
         <rFont val="Avenir"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> meet the criteria &gt;&gt;</t>
     </r>
@@ -138,25 +140,25 @@
   <si>
     <r>
       <rPr>
+        <color theme="1"/>
         <rFont val="Avenir"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">Copy this cell for when you or a competitor </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Avenir"/>
         <i/>
         <color theme="1"/>
+        <rFont val="Avenir"/>
       </rPr>
       <t xml:space="preserve">does not </t>
     </r>
     <r>
       <rPr>
+        <color theme="1"/>
         <rFont val="Avenir"/>
-        <color theme="1"/>
       </rPr>
-      <t>meet the criteria &gt;&gt;</t>
+      <t xml:space="preserve">meet the criteria &gt;&gt;</t>
     </r>
   </si>
   <si>
@@ -166,47 +168,47 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <color indexed="64"/>
+      <sz val="10.000000"/>
     </font>
     <font>
-      <sz val="18.0"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Avenir"/>
+      <color indexed="65"/>
+      <sz val="18.000000"/>
     </font>
     <font>
-      <sz val="14.0"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Avenir"/>
+      <color indexed="65"/>
+      <sz val="14.000000"/>
     </font>
     <font>
+      <name val="Avenir"/>
       <color theme="1"/>
-      <name val="Avenir"/>
     </font>
     <font>
+      <name val="Avenir"/>
       <i/>
       <color theme="1"/>
-      <name val="Avenir"/>
     </font>
     <font>
-      <sz val="18.0"/>
-      <color rgb="FF00BDA5"/>
       <name val="Avenir"/>
+      <b/>
+      <color rgb="FFF2545B"/>
+      <sz val="18.000000"/>
     </font>
     <font>
-      <b/>
-      <sz val="18.0"/>
-      <color rgb="FFF2545B"/>
       <name val="Avenir"/>
+      <color rgb="FF00BDA5"/>
+      <sz val="18.000000"/>
     </font>
     <font>
-      <sz val="18.0"/>
-      <color rgb="FFFF0000"/>
       <name val="Avenir"/>
+      <color indexed="2"/>
+      <sz val="18.000000"/>
     </font>
   </fonts>
   <fills count="6">
@@ -214,7 +216,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -242,66 +244,344 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf fontId="5" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf fontId="6" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf fontId="7" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -358,7 +638,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -384,7 +664,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -436,16 +716,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -461,7 +753,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -491,22 +783,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="47.29"/>
-    <col customWidth="1" min="2" max="2" width="29.14"/>
-    <col customWidth="1" min="3" max="5" width="18.71"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="47.289999999999999"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="29.140000000000001"/>
+    <col bestFit="1" customWidth="1" min="3" max="5" width="18.710000000000001"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -598,14 +894,14 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>7</v>
+      <c r="F5" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -623,6 +919,7 @@
       <c r="T5" s="3"/>
     </row>
     <row r="6">
+      <c r="C6"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -645,17 +942,17 @@
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>7</v>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>7</v>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>7</v>
+      <c r="F7" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -695,17 +992,17 @@
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>7</v>
+      <c r="F9" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -738,24 +1035,24 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" ht="27.0" customHeight="1">
-      <c r="A11" s="10" t="s">
+    <row r="11" ht="27" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>8</v>
+      <c r="E11" s="6" t="s">
+        <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>8</v>
+      <c r="F11" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -772,7 +1069,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" ht="24.0" customHeight="1">
+    <row r="12" ht="24" customHeight="1">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -788,24 +1085,24 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" ht="24.0" customHeight="1">
-      <c r="A13" s="10" t="s">
+    <row r="13" ht="24" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>7</v>
+      <c r="C13" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>7</v>
+      <c r="D13" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
+      <c r="E13" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>7</v>
+      <c r="F13" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -839,23 +1136,23 @@
       <c r="T14" s="3"/>
     </row>
     <row r="15" ht="38.25" customHeight="1">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>8</v>
+      <c r="E15" s="6" t="s">
+        <v>7</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>8</v>
+      <c r="F15" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -889,23 +1186,23 @@
       <c r="T16" s="3"/>
     </row>
     <row r="17" ht="37.5" customHeight="1">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -939,23 +1236,23 @@
       <c r="T18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>7</v>
+      <c r="C19" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>7</v>
+      <c r="D19" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>7</v>
+      <c r="E19" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>7</v>
+      <c r="F19" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -989,23 +1286,23 @@
       <c r="T20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="F21" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1039,23 +1336,23 @@
       <c r="T22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>8</v>
+      <c r="F23" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1089,23 +1386,23 @@
       <c r="T24" s="3"/>
     </row>
     <row r="25" ht="7.5" customHeight="1">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>8</v>
+      <c r="F25" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1139,23 +1436,23 @@
       <c r="T26" s="3"/>
     </row>
     <row r="27" ht="6.75" customHeight="1">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>8</v>
+      <c r="F27" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1195,17 +1492,17 @@
       <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>7</v>
+      <c r="C29" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>7</v>
+      <c r="D29" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>7</v>
+      <c r="E29" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>7</v>
+      <c r="F29" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1254,7 +1551,7 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" ht="21.0" customHeight="1">
+    <row r="32" ht="21" customHeight="1">
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -1397,11 +1694,11 @@
       <c r="T39" s="3"/>
     </row>
     <row r="40">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>7</v>
+      <c r="B40" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1443,11 +1740,11 @@
       <c r="T41" s="3"/>
     </row>
     <row r="42">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>8</v>
+      <c r="B42" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1489,7 +1786,7 @@
       <c r="T43" s="3"/>
     </row>
     <row r="44">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="3"/>
@@ -1513,7 +1810,7 @@
       <c r="T44" s="3"/>
     </row>
     <row r="45">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B45" s="3"/>
@@ -22636,14 +22933,47 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
@@ -22651,29 +22981,29 @@
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="F25:F26"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
@@ -22681,49 +23011,19 @@
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="F29:F30"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>